<commit_message>
updated data for 4/9/2019
</commit_message>
<xml_diff>
--- a/librelink/Rik Activity 2019.xlsx
+++ b/librelink/Rik Activity 2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="576" documentId="13_ncr:1_{A1AD52F5-5758-0A44-8A5A-0AE3A9C1C771}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{6CC8EAFF-744A-9C40-A91B-C396BB6FE602}"/>
+  <xr:revisionPtr revIDLastSave="608" documentId="13_ncr:1_{A1AD52F5-5758-0A44-8A5A-0AE3A9C1C771}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2C82A6D2-701C-A44B-BFCC-B52F943B62EB}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
+    <workbookView xWindow="3400" yWindow="1600" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="166">
   <si>
     <t>Start</t>
   </si>
@@ -515,6 +515,21 @@
   </si>
   <si>
     <t>Banana bread</t>
+  </si>
+  <si>
+    <t>Pizza + breaded chicken</t>
+  </si>
+  <si>
+    <t>Whole wheat pasta</t>
+  </si>
+  <si>
+    <t>eggs + cheese</t>
+  </si>
+  <si>
+    <t>egg/banana/fiber</t>
+  </si>
+  <si>
+    <t>Beans + cabbage</t>
   </si>
 </sst>
 </file>
@@ -764,8 +779,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E190" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:E190" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E201" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:E201" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
     <sortCondition ref="A1:A123"/>
   </sortState>
@@ -1092,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BBD169-48D2-8F48-8801-52F9E2F03988}">
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="A191" sqref="A191"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3962,6 +3977,171 @@
         <v>25</v>
       </c>
       <c r="E190" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>43561.941469907404</v>
+      </c>
+      <c r="B191" s="1">
+        <v>43562.167361111111</v>
+      </c>
+      <c r="C191" t="s">
+        <v>6</v>
+      </c>
+      <c r="E191" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.4213888889644295</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>43561.8125</v>
+      </c>
+      <c r="C192" t="s">
+        <v>4</v>
+      </c>
+      <c r="D192" t="s">
+        <v>161</v>
+      </c>
+      <c r="E192" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>43562.180555555555</v>
+      </c>
+      <c r="C193" t="s">
+        <v>4</v>
+      </c>
+      <c r="D193" t="s">
+        <v>5</v>
+      </c>
+      <c r="E193" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>43561.520833333336</v>
+      </c>
+      <c r="C194" t="s">
+        <v>4</v>
+      </c>
+      <c r="D194" t="s">
+        <v>162</v>
+      </c>
+      <c r="E194" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>43562.40625</v>
+      </c>
+      <c r="C195" t="s">
+        <v>4</v>
+      </c>
+      <c r="D195" t="s">
+        <v>163</v>
+      </c>
+      <c r="E195" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>43563.40625</v>
+      </c>
+      <c r="C196" t="s">
+        <v>4</v>
+      </c>
+      <c r="D196" t="s">
+        <v>164</v>
+      </c>
+      <c r="E196" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>43563.791666666664</v>
+      </c>
+      <c r="C197" t="s">
+        <v>4</v>
+      </c>
+      <c r="D197" t="s">
+        <v>165</v>
+      </c>
+      <c r="E197" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>43563.583333333336</v>
+      </c>
+      <c r="C198" t="s">
+        <v>4</v>
+      </c>
+      <c r="D198" t="s">
+        <v>131</v>
+      </c>
+      <c r="E198" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>43562.939583333333</v>
+      </c>
+      <c r="B199" s="1">
+        <v>43563.228472222225</v>
+      </c>
+      <c r="C199" t="s">
+        <v>6</v>
+      </c>
+      <c r="E199" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.933333333407063</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>43563.90761574074</v>
+      </c>
+      <c r="B200" s="1">
+        <v>43564.199305555558</v>
+      </c>
+      <c r="C200" t="s">
+        <v>6</v>
+      </c>
+      <c r="E200" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.0005555556272157</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>43564.21875</v>
+      </c>
+      <c r="C201" t="s">
+        <v>4</v>
+      </c>
+      <c r="D201" t="s">
+        <v>5</v>
+      </c>
+      <c r="E201" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
         <v>NA</v>
       </c>

</xml_diff>

<commit_message>
Data updates Jul 19
</commit_message>
<xml_diff>
--- a/librelink/Rik Activity 2019.xlsx
+++ b/librelink/Rik Activity 2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="608" documentId="13_ncr:1_{A1AD52F5-5758-0A44-8A5A-0AE3A9C1C771}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2C82A6D2-701C-A44B-BFCC-B52F943B62EB}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{353828E4-0255-2243-A8E5-E6EA79AF6C53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{39AEA28B-D02F-B641-910C-2A5C5D51BA13}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1600" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
+    <workbookView xWindow="400" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="252">
   <si>
     <t>Start</t>
   </si>
@@ -530,12 +530,273 @@
   </si>
   <si>
     <t>Beans + cabbage</t>
+  </si>
+  <si>
+    <t>Chocolate shake</t>
+  </si>
+  <si>
+    <t>Protein Cacao Smoothie</t>
+  </si>
+  <si>
+    <t>Ravioli spinach</t>
+  </si>
+  <si>
+    <t>McDonalds Hamburger</t>
+  </si>
+  <si>
+    <t>Bulletproof bar</t>
+  </si>
+  <si>
+    <t>Burmese tofu salad</t>
+  </si>
+  <si>
+    <t>Acai bowl</t>
+  </si>
+  <si>
+    <t>Cinnamon roll + creamy coffee</t>
+  </si>
+  <si>
+    <t>Lemonade + Chips</t>
+  </si>
+  <si>
+    <t>Ginger Drink</t>
+  </si>
+  <si>
+    <t>Sushi + Udon</t>
+  </si>
+  <si>
+    <t>Protein bar</t>
+  </si>
+  <si>
+    <t>Airplane</t>
+  </si>
+  <si>
+    <t>Pastrami sandwich</t>
+  </si>
+  <si>
+    <t>Chinese rice, noodles, eggs, pork</t>
+  </si>
+  <si>
+    <t>Mushroom chips</t>
+  </si>
+  <si>
+    <t>Chicken, white bread, cheese</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Latte</t>
+  </si>
+  <si>
+    <t>Pork sandwich</t>
+  </si>
+  <si>
+    <t>Coconut rice + beef</t>
+  </si>
+  <si>
+    <t>Rice + Sushi + chicken</t>
+  </si>
+  <si>
+    <t>Beans + kombucha</t>
+  </si>
+  <si>
+    <t>Latte (Almond milk)</t>
+  </si>
+  <si>
+    <t>Beans + Chips</t>
+  </si>
+  <si>
+    <t>FibeRx Smoothie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pizza + Sprite</t>
+  </si>
+  <si>
+    <t>Pea soup</t>
+  </si>
+  <si>
+    <t>Salmon + coconut rice</t>
+  </si>
+  <si>
+    <t>coconut cookie</t>
+  </si>
+  <si>
+    <t>Granola cereal w/milk</t>
+  </si>
+  <si>
+    <t>Tamale</t>
+  </si>
+  <si>
+    <t>Mixed nuts</t>
+  </si>
+  <si>
+    <t>Mushrooms + Broccoli</t>
+  </si>
+  <si>
+    <t>Granola cereal w/milk (Reducose)</t>
+  </si>
+  <si>
+    <t>Salmon + coconut rice (Reducose)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blueberry almond smoothie </t>
+  </si>
+  <si>
+    <t>chips and guacamole</t>
+  </si>
+  <si>
+    <t>Egg tortilla</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>Roast Chicken + Beer</t>
+  </si>
+  <si>
+    <t>Salmon pasta</t>
+  </si>
+  <si>
+    <t>Clams + wine</t>
+  </si>
+  <si>
+    <t>Oatmeal (Reducose)</t>
+  </si>
+  <si>
+    <t>Chicken + Tamale</t>
+  </si>
+  <si>
+    <t>Smoothie (almond milk + banana)</t>
+  </si>
+  <si>
+    <t>Pork Belly + Chips + beans</t>
+  </si>
+  <si>
+    <t>Coconut cookie</t>
+  </si>
+  <si>
+    <t>Pork belly + seeds</t>
+  </si>
+  <si>
+    <t>CBD Chocolate</t>
+  </si>
+  <si>
+    <t>Mushroom bok choy</t>
+  </si>
+  <si>
+    <t>Blueberry smoothie (Reducose)</t>
+  </si>
+  <si>
+    <t>Eggs + avocado</t>
+  </si>
+  <si>
+    <t>banana + breakfast</t>
+  </si>
+  <si>
+    <t>Banana (Reducose T-10)</t>
+  </si>
+  <si>
+    <t>Reducose</t>
+  </si>
+  <si>
+    <t>Chips</t>
+  </si>
+  <si>
+    <t>Biking</t>
+  </si>
+  <si>
+    <t>Burger (0 reducose)</t>
+  </si>
+  <si>
+    <t>Burger (1 hr after chips)</t>
+  </si>
+  <si>
+    <t>Burger (Reducose + 4 hrs)</t>
+  </si>
+  <si>
+    <t>Pork + Nopales</t>
+  </si>
+  <si>
+    <t>Scautoma</t>
+  </si>
+  <si>
+    <t>Apple pastry + Latte</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>Yogurt</t>
+  </si>
+  <si>
+    <t>Chips (Reducose)</t>
+  </si>
+  <si>
+    <t>Blueberry cobbler</t>
+  </si>
+  <si>
+    <t>Pizza (Shrimp-Chorizo)</t>
+  </si>
+  <si>
+    <t>Corn bread</t>
+  </si>
+  <si>
+    <t>Latte + scone</t>
+  </si>
+  <si>
+    <t>Ham sandwich</t>
+  </si>
+  <si>
+    <t>Chicken wings</t>
+  </si>
+  <si>
+    <t>Apple fritter</t>
+  </si>
+  <si>
+    <t>Lemonade</t>
+  </si>
+  <si>
+    <t>Ice cream</t>
+  </si>
+  <si>
+    <t>English muffin</t>
+  </si>
+  <si>
+    <t>English muffin w/egg</t>
+  </si>
+  <si>
+    <t>Cantaloupe</t>
+  </si>
+  <si>
+    <t>Canoli</t>
+  </si>
+  <si>
+    <t>Donut</t>
+  </si>
+  <si>
+    <t>Sausage, bread</t>
+  </si>
+  <si>
+    <t>Salad w/ham</t>
+  </si>
+  <si>
+    <t>Smoothie (Yogurt + Peaches)</t>
+  </si>
+  <si>
+    <t>Chicken + rice</t>
+  </si>
+  <si>
+    <t>Fig bar</t>
+  </si>
+  <si>
+    <t>Peanut butter cookie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -586,7 +847,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -684,11 +945,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -713,6 +983,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,10 +1057,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E201" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:E201" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
-    <sortCondition ref="A1:A123"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E364" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:E364" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E360">
+    <sortCondition ref="A1:A360"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{378B7070-ADA2-F840-857A-A5C12E2181D6}" name="Start" dataDxfId="2"/>
@@ -1107,17 +1385,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BBD169-48D2-8F48-8801-52F9E2F03988}">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="A365" sqref="A365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1421,7 +1699,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="E20" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2798,13 +3076,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>43550.543749999997</v>
+        <v>43549.75</v>
       </c>
       <c r="C112" t="s">
         <v>4</v>
       </c>
       <c r="D112" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="E112" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2813,13 +3091,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>43549.75</v>
+        <v>43549.770833333336</v>
       </c>
       <c r="C113" t="s">
         <v>4</v>
       </c>
       <c r="D113" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="E113" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2828,28 +3106,28 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>43550.754861111112</v>
+        <v>43549.893182870372</v>
+      </c>
+      <c r="B114" s="1">
+        <v>43550.238194444442</v>
       </c>
       <c r="C114" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" t="s">
-        <v>107</v>
-      </c>
-      <c r="E114" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E114" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.2802777776960284</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>43549.770833333336</v>
+        <v>43550.270833333336</v>
       </c>
       <c r="C115" t="s">
         <v>4</v>
       </c>
       <c r="D115" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="E115" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2858,28 +3136,28 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>43549.893182870372</v>
-      </c>
-      <c r="B116" s="1">
-        <v>43550.238194444442</v>
+        <v>43550.385416666664</v>
       </c>
       <c r="C116" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>8.2802777776960284</v>
+        <v>4</v>
+      </c>
+      <c r="D116" t="s">
+        <v>127</v>
+      </c>
+      <c r="E116" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>43550.270833333336</v>
+        <v>43550.543749999997</v>
       </c>
       <c r="C117" t="s">
         <v>4</v>
       </c>
       <c r="D117" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="E117" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2888,13 +3166,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>43550.385416666664</v>
+        <v>43550.754861111112</v>
       </c>
       <c r="C118" t="s">
         <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="E118" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2903,43 +3181,43 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>43550.919282407405</v>
-      </c>
-      <c r="B119" s="1">
-        <v>43551.241666666669</v>
+        <v>43550.781944444447</v>
       </c>
       <c r="C119" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>7.7372222223202698</v>
+        <v>4</v>
+      </c>
+      <c r="D119" t="s">
+        <v>129</v>
+      </c>
+      <c r="E119" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>43551.25</v>
+        <v>43550.919282407405</v>
+      </c>
+      <c r="B120" s="1">
+        <v>43551.241666666669</v>
       </c>
       <c r="C120" t="s">
-        <v>4</v>
-      </c>
-      <c r="D120" t="s">
-        <v>5</v>
-      </c>
-      <c r="E120" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E120" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.7372222223202698</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>43551.375</v>
+        <v>43551.25</v>
       </c>
       <c r="C121" t="s">
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="E121" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2948,13 +3226,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>43551.475694444445</v>
+        <v>43551.375</v>
       </c>
       <c r="C122" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
       <c r="E122" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2963,13 +3241,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>43551.523611111108</v>
+        <v>43551.475694444445</v>
       </c>
       <c r="C123" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D123" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E123" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -2978,13 +3256,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>43550.781944444447</v>
+        <v>43551.523611111108</v>
       </c>
       <c r="C124" t="s">
         <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E124" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3083,17 +3361,17 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>43552.921296296299</v>
-      </c>
-      <c r="B131" s="1">
-        <v>43553.206944444442</v>
+        <v>43552.53125</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
-      </c>
-      <c r="E131" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>6.8555555554339662</v>
+        <v>4</v>
+      </c>
+      <c r="D131" t="s">
+        <v>134</v>
+      </c>
+      <c r="E131" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -3128,17 +3406,17 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>43552.53125</v>
+        <v>43552.921296296299</v>
+      </c>
+      <c r="B134" s="1">
+        <v>43553.206944444442</v>
       </c>
       <c r="C134" t="s">
-        <v>4</v>
-      </c>
-      <c r="D134" t="s">
-        <v>134</v>
-      </c>
-      <c r="E134" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E134" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.8555555554339662</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -3158,28 +3436,28 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>43553.925902777781</v>
-      </c>
-      <c r="B136" s="1">
-        <v>43554.180555555555</v>
+        <v>43553.479166666664</v>
       </c>
       <c r="C136" t="s">
-        <v>6</v>
-      </c>
-      <c r="E136" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>6.1116666665766388</v>
+        <v>4</v>
+      </c>
+      <c r="D136" t="s">
+        <v>140</v>
+      </c>
+      <c r="E136" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>43554.229166666664</v>
+        <v>43553.643055555556</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
       </c>
       <c r="D137" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="E137" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3188,13 +3466,13 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>43553.643055555556</v>
+        <v>43553.75277777778</v>
       </c>
       <c r="C138" t="s">
         <v>4</v>
       </c>
       <c r="D138" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E138" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3203,13 +3481,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>43553.75277777778</v>
+        <v>43553.836111111108</v>
       </c>
       <c r="C139" t="s">
         <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E139" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3218,28 +3496,28 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>43553.836111111108</v>
+        <v>43553.925902777781</v>
+      </c>
+      <c r="B140" s="1">
+        <v>43554.180555555555</v>
       </c>
       <c r="C140" t="s">
-        <v>4</v>
-      </c>
-      <c r="D140" t="s">
-        <v>139</v>
-      </c>
-      <c r="E140" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E140" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.1116666665766388</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>43553.479166666664</v>
+        <v>43554.229166666664</v>
       </c>
       <c r="C141" t="s">
         <v>4</v>
       </c>
       <c r="D141" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="E141" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3248,13 +3526,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>43554.815972222219</v>
+        <v>43554.303472222222</v>
       </c>
       <c r="C142" t="s">
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E142" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3263,28 +3541,28 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>43554.92428240741</v>
-      </c>
-      <c r="B143" s="1">
-        <v>43555.243055555555</v>
+        <v>43554.520138888889</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
-      </c>
-      <c r="E143" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>7.6505555554758757</v>
+        <v>4</v>
+      </c>
+      <c r="D143" t="s">
+        <v>143</v>
+      </c>
+      <c r="E143" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>43554.802777777775</v>
+        <v>43554.708333333336</v>
       </c>
       <c r="C144" t="s">
         <v>4</v>
       </c>
       <c r="D144" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E144" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3293,13 +3571,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>43554.303472222222</v>
+        <v>43554.802777777775</v>
       </c>
       <c r="C145" t="s">
         <v>4</v>
       </c>
       <c r="D145" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="E145" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3308,13 +3586,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>43554.520138888889</v>
+        <v>43554.815972222219</v>
       </c>
       <c r="C146" t="s">
         <v>4</v>
       </c>
       <c r="D146" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E146" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3323,28 +3601,28 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>43555.284722222219</v>
+        <v>43554.92428240741</v>
+      </c>
+      <c r="B147" s="1">
+        <v>43555.243055555555</v>
       </c>
       <c r="C147" t="s">
-        <v>4</v>
-      </c>
-      <c r="D147" t="s">
-        <v>5</v>
-      </c>
-      <c r="E147" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E147" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.6505555554758757</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>43554.708333333336</v>
+        <v>43555.284722222219</v>
       </c>
       <c r="C148" t="s">
         <v>4</v>
       </c>
       <c r="D148" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="E148" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3488,28 +3766,28 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>43556.917546296296</v>
-      </c>
-      <c r="B158" s="1">
-        <v>43557.220833333333</v>
+        <v>43556.708333333336</v>
       </c>
       <c r="C158" t="s">
-        <v>6</v>
-      </c>
-      <c r="E158" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>7.2788888888899237</v>
+        <v>4</v>
+      </c>
+      <c r="D158" t="s">
+        <v>149</v>
+      </c>
+      <c r="E158" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>43557.270833333336</v>
+        <v>43556.78125</v>
       </c>
       <c r="C159" t="s">
         <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="E159" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3518,28 +3796,28 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>43556.78125</v>
+        <v>43556.917546296296</v>
+      </c>
+      <c r="B160" s="1">
+        <v>43557.220833333333</v>
       </c>
       <c r="C160" t="s">
-        <v>4</v>
-      </c>
-      <c r="D160" t="s">
-        <v>148</v>
-      </c>
-      <c r="E160" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E160" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.2788888888899237</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>43556.708333333336</v>
+        <v>43557.270833333336</v>
       </c>
       <c r="C161" t="s">
         <v>4</v>
       </c>
       <c r="D161" t="s">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="E161" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3593,13 +3871,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>43557.886805555558</v>
+        <v>43557.718055555553</v>
       </c>
       <c r="C165" t="s">
         <v>4</v>
       </c>
       <c r="D165" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="E165" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3608,32 +3886,32 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>43557.928136574075</v>
-      </c>
-      <c r="B166" s="1">
-        <v>43558.270138888889</v>
+        <v>43557.886805555558</v>
       </c>
       <c r="C166" t="s">
-        <v>6</v>
-      </c>
-      <c r="E166" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>8.2080555555294268</v>
+        <v>4</v>
+      </c>
+      <c r="D166" t="s">
+        <v>152</v>
+      </c>
+      <c r="E166" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>43557.718055555553</v>
+        <v>43557.928136574075</v>
+      </c>
+      <c r="B167" s="1">
+        <v>43558.270138888889</v>
       </c>
       <c r="C167" t="s">
-        <v>4</v>
-      </c>
-      <c r="D167" t="s">
-        <v>121</v>
-      </c>
-      <c r="E167" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E167" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.2080555555294268</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -3698,43 +3976,43 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>43558.934108796297</v>
-      </c>
-      <c r="B172" s="1">
-        <v>43559.220138888886</v>
+        <v>43558.78125</v>
       </c>
       <c r="C172" t="s">
-        <v>6</v>
-      </c>
-      <c r="E172" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>6.8647222221479751</v>
+        <v>4</v>
+      </c>
+      <c r="D172" t="s">
+        <v>154</v>
+      </c>
+      <c r="E172" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>43559.260416666664</v>
+        <v>43558.934108796297</v>
+      </c>
+      <c r="B173" s="1">
+        <v>43559.220138888886</v>
       </c>
       <c r="C173" t="s">
-        <v>4</v>
-      </c>
-      <c r="D173" t="s">
-        <v>5</v>
-      </c>
-      <c r="E173" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E173" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.8647222221479751</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>43558.78125</v>
+        <v>43559.260416666664</v>
       </c>
       <c r="C174" t="s">
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>154</v>
+        <v>5</v>
       </c>
       <c r="E174" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3758,13 +4036,13 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>43559.53125</v>
+        <v>43559.423611111109</v>
       </c>
       <c r="C176" t="s">
         <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>154</v>
+        <v>77</v>
       </c>
       <c r="E176" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3773,13 +4051,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>43559.635416666664</v>
+        <v>43559.53125</v>
       </c>
       <c r="C177" t="s">
         <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="E177" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3803,13 +4081,13 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>43559.423611111109</v>
+        <v>43559.635416666664</v>
       </c>
       <c r="C179" t="s">
         <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="E179" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3818,43 +4096,43 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>43559.946979166663</v>
-      </c>
-      <c r="B180" s="1">
-        <v>43560.223611111112</v>
+        <v>43559.770833333336</v>
       </c>
       <c r="C180" t="s">
-        <v>6</v>
-      </c>
-      <c r="E180" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>6.6391666667768732</v>
+        <v>4</v>
+      </c>
+      <c r="D180" t="s">
+        <v>157</v>
+      </c>
+      <c r="E180" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>43560.25</v>
+        <v>43559.946979166663</v>
+      </c>
+      <c r="B181" s="1">
+        <v>43560.223611111112</v>
       </c>
       <c r="C181" t="s">
-        <v>4</v>
-      </c>
-      <c r="D181" t="s">
-        <v>5</v>
-      </c>
-      <c r="E181" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E181" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.6391666667768732</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>43560.34375</v>
+        <v>43560.25</v>
       </c>
       <c r="C182" t="s">
         <v>4</v>
       </c>
       <c r="D182" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="E182" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3863,13 +4141,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>43559.770833333336</v>
+        <v>43560.34375</v>
       </c>
       <c r="C183" t="s">
         <v>4</v>
       </c>
       <c r="D183" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E183" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3878,28 +4156,28 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>43560.911620370367</v>
-      </c>
-      <c r="B184" s="1">
-        <v>43561.21875</v>
+        <v>43560.520833333336</v>
       </c>
       <c r="C184" t="s">
-        <v>6</v>
-      </c>
-      <c r="E184" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>7.371111111191567</v>
+        <v>4</v>
+      </c>
+      <c r="D184" t="s">
+        <v>159</v>
+      </c>
+      <c r="E184" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>43560.8125</v>
+        <v>43560.604166666664</v>
       </c>
       <c r="C185" t="s">
         <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E185" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3908,13 +4186,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>43560.520833333336</v>
+        <v>43560.6875</v>
       </c>
       <c r="C186" t="s">
         <v>4</v>
       </c>
       <c r="D186" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E186" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3923,13 +4201,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>43560.604166666664</v>
+        <v>43560.8125</v>
       </c>
       <c r="C187" t="s">
         <v>4</v>
       </c>
       <c r="D187" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E187" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -3938,17 +4216,17 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>43560.6875</v>
+        <v>43560.911620370367</v>
+      </c>
+      <c r="B188" s="1">
+        <v>43561.21875</v>
       </c>
       <c r="C188" t="s">
-        <v>4</v>
-      </c>
-      <c r="D188" t="s">
-        <v>160</v>
-      </c>
-      <c r="E188" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E188" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.371111111191567</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -3983,17 +4261,17 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>43561.941469907404</v>
-      </c>
-      <c r="B191" s="1">
-        <v>43562.167361111111</v>
+        <v>43561.520833333336</v>
       </c>
       <c r="C191" t="s">
-        <v>6</v>
-      </c>
-      <c r="E191" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>5.4213888889644295</v>
+        <v>4</v>
+      </c>
+      <c r="D191" t="s">
+        <v>162</v>
+      </c>
+      <c r="E191" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -4013,28 +4291,28 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>43562.180555555555</v>
+        <v>43561.941469907404</v>
+      </c>
+      <c r="B193" s="1">
+        <v>43562.167361111111</v>
       </c>
       <c r="C193" t="s">
-        <v>4</v>
-      </c>
-      <c r="D193" t="s">
-        <v>5</v>
-      </c>
-      <c r="E193" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E193" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.4213888889644295</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>43561.520833333336</v>
+        <v>43562.180555555555</v>
       </c>
       <c r="C194" t="s">
         <v>4</v>
       </c>
       <c r="D194" t="s">
-        <v>162</v>
+        <v>5</v>
       </c>
       <c r="E194" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -4058,28 +4336,28 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>43563.40625</v>
+        <v>43562.939583333333</v>
+      </c>
+      <c r="B196" s="1">
+        <v>43563.228472222225</v>
       </c>
       <c r="C196" t="s">
-        <v>4</v>
-      </c>
-      <c r="D196" t="s">
-        <v>164</v>
-      </c>
-      <c r="E196" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>NA</v>
+        <v>6</v>
+      </c>
+      <c r="E196" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.933333333407063</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>43563.791666666664</v>
+        <v>43563.40625</v>
       </c>
       <c r="C197" t="s">
         <v>4</v>
       </c>
       <c r="D197" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E197" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -4103,17 +4381,17 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>43562.939583333333</v>
-      </c>
-      <c r="B199" s="1">
-        <v>43563.228472222225</v>
+        <v>43563.791666666664</v>
       </c>
       <c r="C199" t="s">
-        <v>6</v>
-      </c>
-      <c r="E199" s="15">
-        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
-        <v>6.933333333407063</v>
+        <v>4</v>
+      </c>
+      <c r="D199" t="s">
+        <v>165</v>
+      </c>
+      <c r="E199" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -4142,6 +4420,2461 @@
         <v>5</v>
       </c>
       <c r="E201" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>43564.40347222222</v>
+      </c>
+      <c r="C202" t="s">
+        <v>4</v>
+      </c>
+      <c r="D202" t="s">
+        <v>170</v>
+      </c>
+      <c r="E202" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>43564.510416666664</v>
+      </c>
+      <c r="C203" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" t="s">
+        <v>169</v>
+      </c>
+      <c r="E203" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>43564.541666666664</v>
+      </c>
+      <c r="C204" t="s">
+        <v>4</v>
+      </c>
+      <c r="D204" t="s">
+        <v>171</v>
+      </c>
+      <c r="E204" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>43564.802083333336</v>
+      </c>
+      <c r="C205" t="s">
+        <v>4</v>
+      </c>
+      <c r="D205" t="s">
+        <v>168</v>
+      </c>
+      <c r="E205" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>43564.84375</v>
+      </c>
+      <c r="C206" t="s">
+        <v>4</v>
+      </c>
+      <c r="D206" t="s">
+        <v>166</v>
+      </c>
+      <c r="E206" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>43564.968530092592</v>
+      </c>
+      <c r="B207" s="1">
+        <v>43565.259722222225</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
+      <c r="E207" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.9886111111845821</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>43565.3125</v>
+      </c>
+      <c r="C208" t="s">
+        <v>4</v>
+      </c>
+      <c r="D208" t="s">
+        <v>5</v>
+      </c>
+      <c r="E208" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>43565.395833333336</v>
+      </c>
+      <c r="C209" t="s">
+        <v>4</v>
+      </c>
+      <c r="D209" t="s">
+        <v>167</v>
+      </c>
+      <c r="E209" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>43565.484027777777</v>
+      </c>
+      <c r="C210" t="s">
+        <v>4</v>
+      </c>
+      <c r="D210" t="s">
+        <v>179</v>
+      </c>
+      <c r="E210" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>43565.848611111112</v>
+      </c>
+      <c r="C211" t="s">
+        <v>4</v>
+      </c>
+      <c r="D211" t="s">
+        <v>180</v>
+      </c>
+      <c r="E211" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>43565.943912037037</v>
+      </c>
+      <c r="B212" s="1">
+        <v>43566.270833333336</v>
+      </c>
+      <c r="C212" t="s">
+        <v>6</v>
+      </c>
+      <c r="E212" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.846111111168284</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>43566.708333333336</v>
+      </c>
+      <c r="C213" t="s">
+        <v>4</v>
+      </c>
+      <c r="D213" t="s">
+        <v>174</v>
+      </c>
+      <c r="E213" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>43566.992789351854</v>
+      </c>
+      <c r="B214" s="1">
+        <v>43567.271527777775</v>
+      </c>
+      <c r="C214" t="s">
+        <v>6</v>
+      </c>
+      <c r="E214" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.689722222101409</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>43567.333333333336</v>
+      </c>
+      <c r="C215" t="s">
+        <v>4</v>
+      </c>
+      <c r="D215" t="s">
+        <v>173</v>
+      </c>
+      <c r="E215" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>43567.618055555555</v>
+      </c>
+      <c r="C216" t="s">
+        <v>4</v>
+      </c>
+      <c r="D216" t="s">
+        <v>172</v>
+      </c>
+      <c r="E216" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>43567.68472222222</v>
+      </c>
+      <c r="C217" t="s">
+        <v>4</v>
+      </c>
+      <c r="D217" t="s">
+        <v>175</v>
+      </c>
+      <c r="E217" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>43567.75</v>
+      </c>
+      <c r="C218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D218" t="s">
+        <v>176</v>
+      </c>
+      <c r="E218" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>43567.84375</v>
+      </c>
+      <c r="C219" t="s">
+        <v>4</v>
+      </c>
+      <c r="D219" t="s">
+        <v>177</v>
+      </c>
+      <c r="E219" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>43567.993055555555</v>
+      </c>
+      <c r="B220" s="1">
+        <v>43568.0625</v>
+      </c>
+      <c r="C220" t="s">
+        <v>30</v>
+      </c>
+      <c r="D220" t="s">
+        <v>178</v>
+      </c>
+      <c r="E220" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>43568.115115740744</v>
+      </c>
+      <c r="B221" s="1">
+        <v>43568.331944444442</v>
+      </c>
+      <c r="C221" t="s">
+        <v>6</v>
+      </c>
+      <c r="E221" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.2038888887618668</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>43568.378472222219</v>
+      </c>
+      <c r="C222" t="s">
+        <v>4</v>
+      </c>
+      <c r="D222" t="s">
+        <v>5</v>
+      </c>
+      <c r="E222" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>43568.520833333336</v>
+      </c>
+      <c r="C223" t="s">
+        <v>4</v>
+      </c>
+      <c r="D223" t="s">
+        <v>182</v>
+      </c>
+      <c r="E223" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>43568.6875</v>
+      </c>
+      <c r="C224" t="s">
+        <v>4</v>
+      </c>
+      <c r="D224" t="s">
+        <v>181</v>
+      </c>
+      <c r="E224" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>43568.75</v>
+      </c>
+      <c r="C225" t="s">
+        <v>4</v>
+      </c>
+      <c r="D225" t="s">
+        <v>110</v>
+      </c>
+      <c r="E225" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>43568.791666666664</v>
+      </c>
+      <c r="C226" t="s">
+        <v>4</v>
+      </c>
+      <c r="D226" t="s">
+        <v>123</v>
+      </c>
+      <c r="E226" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>43568.893101851849</v>
+      </c>
+      <c r="B227" s="1">
+        <v>43569.199305555558</v>
+      </c>
+      <c r="C227" t="s">
+        <v>6</v>
+      </c>
+      <c r="E227" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.3488888890133239</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>43569.215277777781</v>
+      </c>
+      <c r="C228" t="s">
+        <v>4</v>
+      </c>
+      <c r="D228" t="s">
+        <v>183</v>
+      </c>
+      <c r="E228" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>43569.75</v>
+      </c>
+      <c r="C229" t="s">
+        <v>4</v>
+      </c>
+      <c r="D229" t="s">
+        <v>184</v>
+      </c>
+      <c r="E229" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>43569.906261574077</v>
+      </c>
+      <c r="B230" s="1">
+        <v>43570.177083333336</v>
+      </c>
+      <c r="C230" t="s">
+        <v>6</v>
+      </c>
+      <c r="E230" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.499722222215496</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>43570.270833333336</v>
+      </c>
+      <c r="C231" t="s">
+        <v>4</v>
+      </c>
+      <c r="D231" t="s">
+        <v>5</v>
+      </c>
+      <c r="E231" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
+        <v>43570.3125</v>
+      </c>
+      <c r="C232" t="s">
+        <v>4</v>
+      </c>
+      <c r="D232" t="s">
+        <v>57</v>
+      </c>
+      <c r="E232" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>43570.520833333336</v>
+      </c>
+      <c r="C233" t="s">
+        <v>4</v>
+      </c>
+      <c r="D233" t="s">
+        <v>123</v>
+      </c>
+      <c r="E233" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>43570.770833333336</v>
+      </c>
+      <c r="C234" t="s">
+        <v>4</v>
+      </c>
+      <c r="D234" t="s">
+        <v>185</v>
+      </c>
+      <c r="E234" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" s="1">
+        <v>43570.905891203707</v>
+      </c>
+      <c r="B235" s="1">
+        <v>43571.20416666667</v>
+      </c>
+      <c r="C235" t="s">
+        <v>6</v>
+      </c>
+      <c r="E235" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.1586111111100763</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>43571.245138888888</v>
+      </c>
+      <c r="C236" t="s">
+        <v>4</v>
+      </c>
+      <c r="D236" t="s">
+        <v>5</v>
+      </c>
+      <c r="E236" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>43571.5</v>
+      </c>
+      <c r="C237" t="s">
+        <v>4</v>
+      </c>
+      <c r="D237" t="s">
+        <v>186</v>
+      </c>
+      <c r="E237" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>43571.729166666664</v>
+      </c>
+      <c r="C238" t="s">
+        <v>4</v>
+      </c>
+      <c r="D238" t="s">
+        <v>120</v>
+      </c>
+      <c r="E238" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
+        <v>43571.927164351851</v>
+      </c>
+      <c r="B239" s="1">
+        <v>43572.199305555558</v>
+      </c>
+      <c r="C239" t="s">
+        <v>6</v>
+      </c>
+      <c r="E239" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.5313888889504597</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" s="1">
+        <v>43572.270833333336</v>
+      </c>
+      <c r="C240" t="s">
+        <v>4</v>
+      </c>
+      <c r="D240" t="s">
+        <v>5</v>
+      </c>
+      <c r="E240" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241" s="1">
+        <v>43572.375</v>
+      </c>
+      <c r="C241" t="s">
+        <v>4</v>
+      </c>
+      <c r="D241" t="s">
+        <v>90</v>
+      </c>
+      <c r="E241" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" s="1">
+        <v>43572.527777777781</v>
+      </c>
+      <c r="C242" t="s">
+        <v>4</v>
+      </c>
+      <c r="D242" t="s">
+        <v>187</v>
+      </c>
+      <c r="E242" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>43572.78125</v>
+      </c>
+      <c r="C243" t="s">
+        <v>4</v>
+      </c>
+      <c r="D243" t="s">
+        <v>134</v>
+      </c>
+      <c r="E243" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>43572.975983796299</v>
+      </c>
+      <c r="B244" s="1">
+        <v>43573.28402777778</v>
+      </c>
+      <c r="C244" t="s">
+        <v>6</v>
+      </c>
+      <c r="E244" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.3930555555270985</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>43573.291666666664</v>
+      </c>
+      <c r="C245" t="s">
+        <v>4</v>
+      </c>
+      <c r="D245" t="s">
+        <v>188</v>
+      </c>
+      <c r="E245" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>43573.375</v>
+      </c>
+      <c r="C246" t="s">
+        <v>4</v>
+      </c>
+      <c r="D246" t="s">
+        <v>85</v>
+      </c>
+      <c r="E246" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>43573.45208333333</v>
+      </c>
+      <c r="C247" t="s">
+        <v>4</v>
+      </c>
+      <c r="D247" t="s">
+        <v>190</v>
+      </c>
+      <c r="E247" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>43573.519444444442</v>
+      </c>
+      <c r="C248" t="s">
+        <v>4</v>
+      </c>
+      <c r="D248" t="s">
+        <v>189</v>
+      </c>
+      <c r="E248" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>43573.770833333336</v>
+      </c>
+      <c r="C249" t="s">
+        <v>4</v>
+      </c>
+      <c r="D249" t="s">
+        <v>191</v>
+      </c>
+      <c r="E249" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>43573.89707175926</v>
+      </c>
+      <c r="B250" s="1">
+        <v>43574.261805555558</v>
+      </c>
+      <c r="C250" t="s">
+        <v>6</v>
+      </c>
+      <c r="E250" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.7536111111403443</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>43574.900671296295</v>
+      </c>
+      <c r="B251" s="1">
+        <v>43575.267361111109</v>
+      </c>
+      <c r="C251" t="s">
+        <v>6</v>
+      </c>
+      <c r="E251" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.8005555555573665</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" s="24">
+        <v>43575.947222222225</v>
+      </c>
+      <c r="B252" s="24">
+        <v>43576.203472222223</v>
+      </c>
+      <c r="C252" t="s">
+        <v>6</v>
+      </c>
+      <c r="E252" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.1499999999650754</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>43576.229166666664</v>
+      </c>
+      <c r="C253" t="s">
+        <v>4</v>
+      </c>
+      <c r="D253" t="s">
+        <v>188</v>
+      </c>
+      <c r="E253" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" s="1">
+        <v>43576.241666666669</v>
+      </c>
+      <c r="C254" t="s">
+        <v>4</v>
+      </c>
+      <c r="D254" t="s">
+        <v>192</v>
+      </c>
+      <c r="E254" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" s="1">
+        <v>43601.923449074071</v>
+      </c>
+      <c r="B255" s="25">
+        <v>43602.246527777781</v>
+      </c>
+      <c r="C255" t="s">
+        <v>6</v>
+      </c>
+      <c r="E255" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.7538888890412636</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256" s="1">
+        <v>43602.92287037037</v>
+      </c>
+      <c r="B256" s="25">
+        <v>43603.177083333336</v>
+      </c>
+      <c r="C256" t="s">
+        <v>6</v>
+      </c>
+      <c r="E256" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.1011111111729406</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A257" s="1">
+        <v>43603.807233796295</v>
+      </c>
+      <c r="B257" s="25">
+        <v>43604.163888888892</v>
+      </c>
+      <c r="C257" t="s">
+        <v>6</v>
+      </c>
+      <c r="E257" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.559722222329583</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A258" s="1">
+        <v>43604.811493055553</v>
+      </c>
+      <c r="B258" s="25">
+        <v>43605.161111111112</v>
+      </c>
+      <c r="C258" t="s">
+        <v>6</v>
+      </c>
+      <c r="E258" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.3908333334256895</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A259" s="1">
+        <v>43605.904861111114</v>
+      </c>
+      <c r="B259" s="25">
+        <v>43606.128472222219</v>
+      </c>
+      <c r="C259" t="s">
+        <v>6</v>
+      </c>
+      <c r="E259" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.3666666665230878</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A260" s="1">
+        <v>43606.28125</v>
+      </c>
+      <c r="C260" t="s">
+        <v>4</v>
+      </c>
+      <c r="D260" t="s">
+        <v>5</v>
+      </c>
+      <c r="E260" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A261" s="1">
+        <v>43606.743055555555</v>
+      </c>
+      <c r="C261" t="s">
+        <v>4</v>
+      </c>
+      <c r="D261" t="s">
+        <v>197</v>
+      </c>
+      <c r="E261" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>43606.851388888892</v>
+      </c>
+      <c r="C262" t="s">
+        <v>4</v>
+      </c>
+      <c r="D262" t="s">
+        <v>196</v>
+      </c>
+      <c r="E262" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>43606.892592592594</v>
+      </c>
+      <c r="B263" s="25">
+        <v>43607.195138888892</v>
+      </c>
+      <c r="C263" t="s">
+        <v>6</v>
+      </c>
+      <c r="E263" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.2611111111473292</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>43607.433333333334</v>
+      </c>
+      <c r="C264" t="s">
+        <v>4</v>
+      </c>
+      <c r="D264" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E264" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>43607.541666666664</v>
+      </c>
+      <c r="C265" t="s">
+        <v>4</v>
+      </c>
+      <c r="D265" t="s">
+        <v>198</v>
+      </c>
+      <c r="E265" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>43607.645833333336</v>
+      </c>
+      <c r="C266" t="s">
+        <v>4</v>
+      </c>
+      <c r="D266" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E266" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>43607.763888888891</v>
+      </c>
+      <c r="C267" t="s">
+        <v>4</v>
+      </c>
+      <c r="D267" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E267" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>43607.907025462962</v>
+      </c>
+      <c r="B268" s="1">
+        <v>43608.226388888892</v>
+      </c>
+      <c r="C268" t="s">
+        <v>6</v>
+      </c>
+      <c r="E268" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.6647222223109566</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>43608.25</v>
+      </c>
+      <c r="C269" t="s">
+        <v>4</v>
+      </c>
+      <c r="D269" t="s">
+        <v>5</v>
+      </c>
+      <c r="E269" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>43608.348611111112</v>
+      </c>
+      <c r="C270" t="s">
+        <v>4</v>
+      </c>
+      <c r="D270" t="s">
+        <v>195</v>
+      </c>
+      <c r="E270" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
+        <v>43608.490277777775</v>
+      </c>
+      <c r="C271" t="s">
+        <v>4</v>
+      </c>
+      <c r="D271" t="s">
+        <v>200</v>
+      </c>
+      <c r="E271" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>43608.581944444442</v>
+      </c>
+      <c r="C272" t="s">
+        <v>4</v>
+      </c>
+      <c r="D272" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E272" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
+        <v>43608.600694444445</v>
+      </c>
+      <c r="C273" t="s">
+        <v>4</v>
+      </c>
+      <c r="D273" t="s">
+        <v>202</v>
+      </c>
+      <c r="E273" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>43608.770833333336</v>
+      </c>
+      <c r="C274" t="s">
+        <v>4</v>
+      </c>
+      <c r="D274" t="s">
+        <v>122</v>
+      </c>
+      <c r="E274" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>43608.833333333336</v>
+      </c>
+      <c r="C275" t="s">
+        <v>4</v>
+      </c>
+      <c r="D275" t="s">
+        <v>110</v>
+      </c>
+      <c r="E275" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>43608.894791666666</v>
+      </c>
+      <c r="B276" s="1">
+        <v>43609.125</v>
+      </c>
+      <c r="C276" t="s">
+        <v>6</v>
+      </c>
+      <c r="E276" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.5250000000232831</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>43609.1875</v>
+      </c>
+      <c r="B277" s="1">
+        <v>43609.302083333336</v>
+      </c>
+      <c r="C277" t="s">
+        <v>6</v>
+      </c>
+      <c r="E277" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>2.7500000000582077</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>43609.316666666666</v>
+      </c>
+      <c r="C278" t="s">
+        <v>4</v>
+      </c>
+      <c r="D278" t="s">
+        <v>188</v>
+      </c>
+      <c r="E278" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>43609.416666666664</v>
+      </c>
+      <c r="C279" t="s">
+        <v>4</v>
+      </c>
+      <c r="D279" t="s">
+        <v>203</v>
+      </c>
+      <c r="E279" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>43609.542361111111</v>
+      </c>
+      <c r="C280" t="s">
+        <v>4</v>
+      </c>
+      <c r="D280" t="s">
+        <v>122</v>
+      </c>
+      <c r="E280" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A281" s="28">
+        <v>43609.8</v>
+      </c>
+      <c r="B281" s="3"/>
+      <c r="C281" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D281" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E281" s="27" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>43609.856944444444</v>
+      </c>
+      <c r="C282" t="s">
+        <v>4</v>
+      </c>
+      <c r="D282" t="s">
+        <v>204</v>
+      </c>
+      <c r="E282" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A283" s="29">
+        <v>43609.949594907404</v>
+      </c>
+      <c r="B283" s="1">
+        <v>43610.259722222225</v>
+      </c>
+      <c r="E283" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>43610.270833333336</v>
+      </c>
+      <c r="C284" t="s">
+        <v>4</v>
+      </c>
+      <c r="D284" t="s">
+        <v>188</v>
+      </c>
+      <c r="E284" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>43610.386805555558</v>
+      </c>
+      <c r="C285" t="s">
+        <v>4</v>
+      </c>
+      <c r="D285" t="s">
+        <v>199</v>
+      </c>
+      <c r="E285" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>43610.503472222219</v>
+      </c>
+      <c r="C286" t="s">
+        <v>4</v>
+      </c>
+      <c r="D286" t="s">
+        <v>206</v>
+      </c>
+      <c r="E286" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>43610.557638888888</v>
+      </c>
+      <c r="C287" t="s">
+        <v>4</v>
+      </c>
+      <c r="D287" t="s">
+        <v>194</v>
+      </c>
+      <c r="E287" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
+        <v>43610.786805555559</v>
+      </c>
+      <c r="C288" t="s">
+        <v>4</v>
+      </c>
+      <c r="D288" t="s">
+        <v>207</v>
+      </c>
+      <c r="E288" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
+        <v>43610.923946759256</v>
+      </c>
+      <c r="B289" s="1">
+        <v>43611.249305555553</v>
+      </c>
+      <c r="C289" t="s">
+        <v>6</v>
+      </c>
+      <c r="E289" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.8086111111333594</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>43611.283333333333</v>
+      </c>
+      <c r="C290" t="s">
+        <v>4</v>
+      </c>
+      <c r="D290" t="s">
+        <v>188</v>
+      </c>
+      <c r="E290" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>43611.349305555559</v>
+      </c>
+      <c r="C291" t="s">
+        <v>4</v>
+      </c>
+      <c r="D291" t="s">
+        <v>208</v>
+      </c>
+      <c r="E291" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>43611.477777777778</v>
+      </c>
+      <c r="C292" t="s">
+        <v>4</v>
+      </c>
+      <c r="D292" t="s">
+        <v>212</v>
+      </c>
+      <c r="E292" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>43611.53402777778</v>
+      </c>
+      <c r="C293" t="s">
+        <v>4</v>
+      </c>
+      <c r="D293" t="s">
+        <v>209</v>
+      </c>
+      <c r="E293" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>43611.552083333336</v>
+      </c>
+      <c r="C294" t="s">
+        <v>4</v>
+      </c>
+      <c r="D294" t="s">
+        <v>210</v>
+      </c>
+      <c r="E294" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>43611.755555555559</v>
+      </c>
+      <c r="C295" t="s">
+        <v>4</v>
+      </c>
+      <c r="D295" t="s">
+        <v>211</v>
+      </c>
+      <c r="E295" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A296" s="24">
+        <v>43611.9</v>
+      </c>
+      <c r="B296" s="24">
+        <v>43612.2</v>
+      </c>
+      <c r="C296" t="s">
+        <v>6</v>
+      </c>
+      <c r="E296" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.1999999998952262</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A297" s="24">
+        <v>43612.25</v>
+      </c>
+      <c r="C297" t="s">
+        <v>4</v>
+      </c>
+      <c r="D297" t="s">
+        <v>5</v>
+      </c>
+      <c r="E297" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A298" s="24">
+        <v>43612.3125</v>
+      </c>
+      <c r="C298" t="s">
+        <v>4</v>
+      </c>
+      <c r="D298" t="s">
+        <v>90</v>
+      </c>
+      <c r="E298" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
+        <v>43612.398611111108</v>
+      </c>
+      <c r="C299" t="s">
+        <v>4</v>
+      </c>
+      <c r="D299" t="s">
+        <v>213</v>
+      </c>
+      <c r="E299" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>43612.591666666667</v>
+      </c>
+      <c r="C300" t="s">
+        <v>4</v>
+      </c>
+      <c r="D300" t="s">
+        <v>223</v>
+      </c>
+      <c r="E300" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>43612.642361111109</v>
+      </c>
+      <c r="C301" t="s">
+        <v>4</v>
+      </c>
+      <c r="D301" t="s">
+        <v>216</v>
+      </c>
+      <c r="E301" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>43612.644444444442</v>
+      </c>
+      <c r="C302" t="s">
+        <v>4</v>
+      </c>
+      <c r="D302" t="s">
+        <v>214</v>
+      </c>
+      <c r="E302" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>43612.8125</v>
+      </c>
+      <c r="C303" t="s">
+        <v>4</v>
+      </c>
+      <c r="D303" t="s">
+        <v>215</v>
+      </c>
+      <c r="E303" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>43612.882141203707</v>
+      </c>
+      <c r="B304" s="1">
+        <v>43613.260416666664</v>
+      </c>
+      <c r="C304" t="s">
+        <v>6</v>
+      </c>
+      <c r="E304" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>9.0786111109773628</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>43613.271527777775</v>
+      </c>
+      <c r="C305" t="s">
+        <v>4</v>
+      </c>
+      <c r="D305" t="s">
+        <v>188</v>
+      </c>
+      <c r="E305" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>43613.352083333331</v>
+      </c>
+      <c r="C306" t="s">
+        <v>4</v>
+      </c>
+      <c r="D306" t="s">
+        <v>219</v>
+      </c>
+      <c r="E306" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>43613.431944444441</v>
+      </c>
+      <c r="C307" t="s">
+        <v>4</v>
+      </c>
+      <c r="D307" t="s">
+        <v>217</v>
+      </c>
+      <c r="E307" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A308" s="28">
+        <v>43613.520833333336</v>
+      </c>
+      <c r="B308" s="3"/>
+      <c r="C308" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D308" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E308" s="27" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>43613.767361111109</v>
+      </c>
+      <c r="C309" t="s">
+        <v>4</v>
+      </c>
+      <c r="D309" t="s">
+        <v>134</v>
+      </c>
+      <c r="E309" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>43613.895532407405</v>
+      </c>
+      <c r="B310" s="1">
+        <v>43614.222916666666</v>
+      </c>
+      <c r="C310" t="s">
+        <v>6</v>
+      </c>
+      <c r="E310" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.8572222222574055</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>43614.25</v>
+      </c>
+      <c r="C311" t="s">
+        <v>4</v>
+      </c>
+      <c r="D311" t="s">
+        <v>5</v>
+      </c>
+      <c r="E311" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A312" s="29">
+        <v>43614.314583333333</v>
+      </c>
+      <c r="C312" t="s">
+        <v>4</v>
+      </c>
+      <c r="D312" t="s">
+        <v>220</v>
+      </c>
+      <c r="E312" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A313" s="29">
+        <v>43614.328472222223</v>
+      </c>
+      <c r="C313" t="s">
+        <v>4</v>
+      </c>
+      <c r="D313" t="s">
+        <v>85</v>
+      </c>
+      <c r="E313" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A314" s="29">
+        <v>43614.462500000001</v>
+      </c>
+      <c r="C314" t="s">
+        <v>4</v>
+      </c>
+      <c r="D314" t="s">
+        <v>231</v>
+      </c>
+      <c r="E314" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A315" s="30">
+        <v>43614.529861111114</v>
+      </c>
+      <c r="C315" t="s">
+        <v>4</v>
+      </c>
+      <c r="D315" t="s">
+        <v>224</v>
+      </c>
+      <c r="E315" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316" s="1">
+        <v>43614.570833333331</v>
+      </c>
+      <c r="C316" t="s">
+        <v>4</v>
+      </c>
+      <c r="D316" t="s">
+        <v>110</v>
+      </c>
+      <c r="E316" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317" s="1">
+        <v>43614.577777777777</v>
+      </c>
+      <c r="B317" s="1">
+        <v>43614.586805555555</v>
+      </c>
+      <c r="C317" t="s">
+        <v>7</v>
+      </c>
+      <c r="D317" t="s">
+        <v>222</v>
+      </c>
+      <c r="E317" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A318" s="1">
+        <v>43614.59375</v>
+      </c>
+      <c r="C318" t="s">
+        <v>4</v>
+      </c>
+      <c r="D318" t="s">
+        <v>109</v>
+      </c>
+      <c r="E318" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319" s="1">
+        <v>43614.701388888891</v>
+      </c>
+      <c r="B319" s="1">
+        <v>43614.711805555555</v>
+      </c>
+      <c r="C319" t="s">
+        <v>7</v>
+      </c>
+      <c r="D319" t="s">
+        <v>222</v>
+      </c>
+      <c r="E319" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A320" s="1">
+        <v>43614.71875</v>
+      </c>
+      <c r="C320" t="s">
+        <v>4</v>
+      </c>
+      <c r="D320" t="s">
+        <v>197</v>
+      </c>
+      <c r="E320" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A321" s="1">
+        <v>43614.769444444442</v>
+      </c>
+      <c r="C321" t="s">
+        <v>4</v>
+      </c>
+      <c r="D321" t="s">
+        <v>226</v>
+      </c>
+      <c r="E321" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>43614.774305555555</v>
+      </c>
+      <c r="B322" s="1">
+        <v>43614.795138888891</v>
+      </c>
+      <c r="C322" t="s">
+        <v>30</v>
+      </c>
+      <c r="D322" t="s">
+        <v>227</v>
+      </c>
+      <c r="E322" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>43614.935416666667</v>
+      </c>
+      <c r="B323" s="1">
+        <v>43615.277083333334</v>
+      </c>
+      <c r="C323" t="s">
+        <v>6</v>
+      </c>
+      <c r="E323" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.2000000000116415</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>43615.284722222219</v>
+      </c>
+      <c r="C324" t="s">
+        <v>4</v>
+      </c>
+      <c r="D324" t="s">
+        <v>5</v>
+      </c>
+      <c r="E324" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>43615.502083333333</v>
+      </c>
+      <c r="C325" t="s">
+        <v>4</v>
+      </c>
+      <c r="D325" t="s">
+        <v>221</v>
+      </c>
+      <c r="E325" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A326" s="1">
+        <v>43615.586805555555</v>
+      </c>
+      <c r="C326" t="s">
+        <v>4</v>
+      </c>
+      <c r="D326" t="s">
+        <v>229</v>
+      </c>
+      <c r="E326" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A327" s="1">
+        <v>43615.592361111114</v>
+      </c>
+      <c r="C327" t="s">
+        <v>4</v>
+      </c>
+      <c r="D327" t="s">
+        <v>230</v>
+      </c>
+      <c r="E327" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>43615.777777777781</v>
+      </c>
+      <c r="C328" t="s">
+        <v>4</v>
+      </c>
+      <c r="D328" t="s">
+        <v>182</v>
+      </c>
+      <c r="E328" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>43615.925358796296</v>
+      </c>
+      <c r="B329" s="1">
+        <v>43616.273611111108</v>
+      </c>
+      <c r="C329" t="s">
+        <v>6</v>
+      </c>
+      <c r="E329" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.3580555554945022</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>43616.285416666666</v>
+      </c>
+      <c r="C330" t="s">
+        <v>4</v>
+      </c>
+      <c r="D330" t="s">
+        <v>228</v>
+      </c>
+      <c r="E330" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>43660.386805555558</v>
+      </c>
+      <c r="C331" t="s">
+        <v>4</v>
+      </c>
+      <c r="D331" t="s">
+        <v>232</v>
+      </c>
+      <c r="E331" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>43660.59097222222</v>
+      </c>
+      <c r="C332" t="s">
+        <v>4</v>
+      </c>
+      <c r="D332" t="s">
+        <v>233</v>
+      </c>
+      <c r="E332" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A333" s="1">
+        <v>43660.645833333336</v>
+      </c>
+      <c r="C333" t="s">
+        <v>4</v>
+      </c>
+      <c r="D333" t="s">
+        <v>54</v>
+      </c>
+      <c r="E333" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>43660.920138888891</v>
+      </c>
+      <c r="B334" s="1">
+        <v>43661.230555555558</v>
+      </c>
+      <c r="C334" t="s">
+        <v>6</v>
+      </c>
+      <c r="E334" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.4500000000116415</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>43661.362500000003</v>
+      </c>
+      <c r="C335" t="s">
+        <v>4</v>
+      </c>
+      <c r="D335" t="s">
+        <v>234</v>
+      </c>
+      <c r="E335" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A336" s="1">
+        <v>43661.447916666664</v>
+      </c>
+      <c r="C336" t="s">
+        <v>4</v>
+      </c>
+      <c r="D336" t="s">
+        <v>235</v>
+      </c>
+      <c r="E336" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A337" s="1">
+        <v>43661.534722222219</v>
+      </c>
+      <c r="C337" t="s">
+        <v>4</v>
+      </c>
+      <c r="D337" t="s">
+        <v>236</v>
+      </c>
+      <c r="E337" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A338" s="1">
+        <v>43661.5625</v>
+      </c>
+      <c r="B338" s="1">
+        <v>43661.6875</v>
+      </c>
+      <c r="C338" t="s">
+        <v>7</v>
+      </c>
+      <c r="E338" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A339" s="1">
+        <v>43661.677083333336</v>
+      </c>
+      <c r="C339" t="s">
+        <v>4</v>
+      </c>
+      <c r="D339" t="s">
+        <v>239</v>
+      </c>
+      <c r="E339" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A340" s="1">
+        <v>43661.784722222219</v>
+      </c>
+      <c r="C340" t="s">
+        <v>4</v>
+      </c>
+      <c r="D340" t="s">
+        <v>237</v>
+      </c>
+      <c r="E340" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A341" s="1">
+        <v>43661.916875000003</v>
+      </c>
+      <c r="B341" s="1">
+        <v>43662.204861111109</v>
+      </c>
+      <c r="C341" t="s">
+        <v>6</v>
+      </c>
+      <c r="E341" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.9116666665649973</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A342" s="1">
+        <v>43662.300694444442</v>
+      </c>
+      <c r="C342" t="s">
+        <v>4</v>
+      </c>
+      <c r="D342" t="s">
+        <v>242</v>
+      </c>
+      <c r="E342" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A343" s="1">
+        <v>43662.390972222223</v>
+      </c>
+      <c r="C343" t="s">
+        <v>4</v>
+      </c>
+      <c r="D343" t="s">
+        <v>238</v>
+      </c>
+      <c r="E343" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A344" s="1">
+        <v>43662.451388888891</v>
+      </c>
+      <c r="C344" t="s">
+        <v>4</v>
+      </c>
+      <c r="D344" t="s">
+        <v>240</v>
+      </c>
+      <c r="E344" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A345" s="1">
+        <v>43662.513194444444</v>
+      </c>
+      <c r="C345" t="s">
+        <v>4</v>
+      </c>
+      <c r="D345" t="s">
+        <v>117</v>
+      </c>
+      <c r="E345" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A346" s="1">
+        <v>43662.694444444445</v>
+      </c>
+      <c r="C346" t="s">
+        <v>4</v>
+      </c>
+      <c r="D346" t="s">
+        <v>241</v>
+      </c>
+      <c r="E346" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A347" s="1">
+        <v>43662.754166666666</v>
+      </c>
+      <c r="C347" t="s">
+        <v>4</v>
+      </c>
+      <c r="D347" t="s">
+        <v>134</v>
+      </c>
+      <c r="E347" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A348" s="1">
+        <v>43662.777777777781</v>
+      </c>
+      <c r="C348" t="s">
+        <v>4</v>
+      </c>
+      <c r="D348" t="s">
+        <v>244</v>
+      </c>
+      <c r="E348" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A349" s="1">
+        <v>43662.882395833331</v>
+      </c>
+      <c r="B349" s="1">
+        <v>43663.219444444447</v>
+      </c>
+      <c r="C349" t="s">
+        <v>6</v>
+      </c>
+      <c r="E349" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.0891666667885147</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A350" s="1">
+        <v>43663.244444444441</v>
+      </c>
+      <c r="C350" t="s">
+        <v>4</v>
+      </c>
+      <c r="D350" t="s">
+        <v>243</v>
+      </c>
+      <c r="E350" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A351" s="1">
+        <v>43663.320138888892</v>
+      </c>
+      <c r="C351" t="s">
+        <v>4</v>
+      </c>
+      <c r="D351" t="s">
+        <v>242</v>
+      </c>
+      <c r="E351" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A352" s="1">
+        <v>43663.395138888889</v>
+      </c>
+      <c r="C352" t="s">
+        <v>4</v>
+      </c>
+      <c r="D352" t="s">
+        <v>245</v>
+      </c>
+      <c r="E352" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A353" s="2">
+        <v>43663.409722222219</v>
+      </c>
+      <c r="B353" s="30">
+        <v>43663.430555555555</v>
+      </c>
+      <c r="C353" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D353" s="3"/>
+      <c r="E353" s="27" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A354" s="1">
+        <v>43663.532638888886</v>
+      </c>
+      <c r="C354" t="s">
+        <v>4</v>
+      </c>
+      <c r="D354" t="s">
+        <v>248</v>
+      </c>
+      <c r="E354" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A355" s="1">
+        <v>43663.613194444442</v>
+      </c>
+      <c r="C355" t="s">
+        <v>4</v>
+      </c>
+      <c r="D355" t="s">
+        <v>247</v>
+      </c>
+      <c r="E355" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A356" s="31">
+        <v>43663.8125</v>
+      </c>
+      <c r="C356" t="s">
+        <v>4</v>
+      </c>
+      <c r="D356" t="s">
+        <v>246</v>
+      </c>
+      <c r="E356" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A357" s="24">
+        <v>43663.908333333333</v>
+      </c>
+      <c r="B357" s="24">
+        <v>43664.254861111112</v>
+      </c>
+      <c r="C357" t="s">
+        <v>6</v>
+      </c>
+      <c r="E357" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.3166666667093523</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A358" s="24">
+        <v>43664.311805555553</v>
+      </c>
+      <c r="B358" s="24">
+        <v>43664.351388888892</v>
+      </c>
+      <c r="C358" t="s">
+        <v>6</v>
+      </c>
+      <c r="E358" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>0.95000000012805685</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A359" s="28">
+        <v>43664.375</v>
+      </c>
+      <c r="B359" s="3"/>
+      <c r="C359" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D359" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E359" s="27" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A360" s="1">
+        <v>43664.78125</v>
+      </c>
+      <c r="C360" t="s">
+        <v>4</v>
+      </c>
+      <c r="D360" t="s">
+        <v>249</v>
+      </c>
+      <c r="E360" s="15"/>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A361" s="1">
+        <v>43664.875</v>
+      </c>
+      <c r="B361" s="1">
+        <v>43665.175694444442</v>
+      </c>
+      <c r="C361" t="s">
+        <v>6</v>
+      </c>
+      <c r="E361" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.21666666661622</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A362" s="24">
+        <v>43664.569444444445</v>
+      </c>
+      <c r="B362" s="24">
+        <v>43664.611111111109</v>
+      </c>
+      <c r="C362" t="s">
+        <v>7</v>
+      </c>
+      <c r="E362" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A363" s="1">
+        <v>43664.662499999999</v>
+      </c>
+      <c r="C363" t="s">
+        <v>4</v>
+      </c>
+      <c r="D363" t="s">
+        <v>250</v>
+      </c>
+      <c r="E363" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A364" s="1">
+        <v>43664.497916666667</v>
+      </c>
+      <c r="C364" t="s">
+        <v>4</v>
+      </c>
+      <c r="D364" t="s">
+        <v>251</v>
+      </c>
+      <c r="E364" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
         <v>NA</v>
       </c>

</xml_diff>

<commit_message>
updated data mid-morning 7/27
</commit_message>
<xml_diff>
--- a/librelink/Rik Activity 2019.xlsx
+++ b/librelink/Rik Activity 2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="8_{353828E4-0255-2243-A8E5-E6EA79AF6C53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{C1EED05F-0DCA-5B45-A604-2B2CE2ED1B25}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="8_{353828E4-0255-2243-A8E5-E6EA79AF6C53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D8257C39-101F-1C4A-967B-722455F8853C}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="272">
   <si>
     <t>Start</t>
   </si>
@@ -821,6 +821,33 @@
   </si>
   <si>
     <t>Nuts and Seeds</t>
+  </si>
+  <si>
+    <t>English muffin w/egg strawberry</t>
+  </si>
+  <si>
+    <t>Cod + bread + wine</t>
+  </si>
+  <si>
+    <t>Pad Thai + quinoa</t>
+  </si>
+  <si>
+    <t>Bread + egg</t>
+  </si>
+  <si>
+    <t>Smoothie</t>
+  </si>
+  <si>
+    <t>Beans + salad + seafood + bread</t>
+  </si>
+  <si>
+    <t>Seafood + rice + salad + brownie</t>
+  </si>
+  <si>
+    <t>Salad w/pork belly and bread</t>
+  </si>
+  <si>
+    <t>Cabbage + tofu</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1118,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E390" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:E390" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E410" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:E410" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E360">
     <sortCondition ref="A1:A360"/>
   </sortState>
@@ -1419,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BBD169-48D2-8F48-8801-52F9E2F03988}">
-  <dimension ref="A1:E390"/>
+  <dimension ref="A1:E410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
-      <selection activeCell="D390" sqref="D390"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="A411" sqref="A411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7300,6 +7327,306 @@
         <v>117</v>
       </c>
       <c r="E390" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A391" s="1">
+        <v>43670.357638888891</v>
+      </c>
+      <c r="C391" t="s">
+        <v>4</v>
+      </c>
+      <c r="D391" t="s">
+        <v>263</v>
+      </c>
+      <c r="E391" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A392" s="1">
+        <v>43670.891435185185</v>
+      </c>
+      <c r="B392" s="1">
+        <v>43671.227083333331</v>
+      </c>
+      <c r="C392" t="s">
+        <v>6</v>
+      </c>
+      <c r="E392" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.0555555555038154</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A393" s="1">
+        <v>43670.684027777781</v>
+      </c>
+      <c r="C393" t="s">
+        <v>4</v>
+      </c>
+      <c r="D393" t="s">
+        <v>201</v>
+      </c>
+      <c r="E393" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A394" s="1">
+        <v>43670.78125</v>
+      </c>
+      <c r="C394" t="s">
+        <v>4</v>
+      </c>
+      <c r="D394" t="s">
+        <v>264</v>
+      </c>
+      <c r="E394" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A395" s="1">
+        <v>43670.635416666664</v>
+      </c>
+      <c r="B395" s="1">
+        <v>43670.666666666664</v>
+      </c>
+      <c r="C395" t="s">
+        <v>7</v>
+      </c>
+      <c r="E395" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A396" s="1">
+        <v>43670.53125</v>
+      </c>
+      <c r="B396" s="1">
+        <v>43670.5625</v>
+      </c>
+      <c r="C396" t="s">
+        <v>7</v>
+      </c>
+      <c r="E396" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A397" s="1">
+        <v>43670.5</v>
+      </c>
+      <c r="C397" t="s">
+        <v>4</v>
+      </c>
+      <c r="D397" t="s">
+        <v>265</v>
+      </c>
+      <c r="E397" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A398" s="1">
+        <v>43671.920648148145</v>
+      </c>
+      <c r="B398" s="1">
+        <v>43672.236805555556</v>
+      </c>
+      <c r="C398" t="s">
+        <v>6</v>
+      </c>
+      <c r="E398" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.5877777778659947</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A399" s="1">
+        <v>43671.291666666664</v>
+      </c>
+      <c r="C399" t="s">
+        <v>4</v>
+      </c>
+      <c r="D399" t="s">
+        <v>266</v>
+      </c>
+      <c r="E399" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A400" s="1">
+        <v>43671.322916666664</v>
+      </c>
+      <c r="B400" s="1">
+        <v>43671.354166666664</v>
+      </c>
+      <c r="C400" t="s">
+        <v>7</v>
+      </c>
+      <c r="E400" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A401" s="1">
+        <v>43671.354166666664</v>
+      </c>
+      <c r="C401" t="s">
+        <v>4</v>
+      </c>
+      <c r="D401" t="s">
+        <v>267</v>
+      </c>
+      <c r="E401" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A402" s="1">
+        <v>43671.520833333336</v>
+      </c>
+      <c r="C402" t="s">
+        <v>4</v>
+      </c>
+      <c r="D402" t="s">
+        <v>268</v>
+      </c>
+      <c r="E402" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A403" s="1">
+        <v>43671.791666666664</v>
+      </c>
+      <c r="C403" t="s">
+        <v>4</v>
+      </c>
+      <c r="D403" t="s">
+        <v>269</v>
+      </c>
+      <c r="E403" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A404" s="1">
+        <v>43671.833333333336</v>
+      </c>
+      <c r="B404" s="1">
+        <v>43671.868055555555</v>
+      </c>
+      <c r="C404" t="s">
+        <v>7</v>
+      </c>
+      <c r="E404" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A405" s="1">
+        <v>43672.364583333336</v>
+      </c>
+      <c r="C405" t="s">
+        <v>4</v>
+      </c>
+      <c r="D405" t="s">
+        <v>266</v>
+      </c>
+      <c r="E405" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A406" s="1">
+        <v>43672.770833333336</v>
+      </c>
+      <c r="C406" t="s">
+        <v>4</v>
+      </c>
+      <c r="D406" t="s">
+        <v>270</v>
+      </c>
+      <c r="E406" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A407" s="1">
+        <v>43672.510416666664</v>
+      </c>
+      <c r="C407" t="s">
+        <v>4</v>
+      </c>
+      <c r="D407" t="s">
+        <v>271</v>
+      </c>
+      <c r="E407" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A408" s="24">
+        <v>43672.909722222219</v>
+      </c>
+      <c r="B408" s="24">
+        <v>43673.236111111109</v>
+      </c>
+      <c r="C408" t="s">
+        <v>6</v>
+      </c>
+      <c r="E408" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.8333333333721384</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A409" s="1">
+        <v>43672.409722222219</v>
+      </c>
+      <c r="B409" s="1">
+        <v>43672.420138888891</v>
+      </c>
+      <c r="C409" t="s">
+        <v>7</v>
+      </c>
+      <c r="E409" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A410" s="1">
+        <v>43673.28125</v>
+      </c>
+      <c r="C410" t="s">
+        <v>4</v>
+      </c>
+      <c r="D410" t="s">
+        <v>241</v>
+      </c>
+      <c r="E410" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
         <v>NA</v>
       </c>

</xml_diff>

<commit_message>
updated data thru 2019-11-04 new function food_auc() to calculate AUC
</commit_message>
<xml_diff>
--- a/librelink/Rik Activity 2019.xlsx
+++ b/librelink/Rik Activity 2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="592" documentId="114_{B7357B50-4B94-C145-ACEA-929B2CB5DE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49455FC6-252B-AD47-8E59-961C9EFD4744}"/>
+  <xr:revisionPtr revIDLastSave="720" documentId="114_{B7357B50-4B94-C145-ACEA-929B2CB5DE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C09E1073-8039-CF4B-9841-08FD33A31227}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="2080" windowWidth="28040" windowHeight="17540" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
+    <workbookView xWindow="4000" yWindow="1240" windowWidth="28040" windowHeight="17540" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="429">
   <si>
     <t>Start</t>
   </si>
@@ -1250,6 +1250,75 @@
   </si>
   <si>
     <t>Granola (90g) almond milk + banana</t>
+  </si>
+  <si>
+    <t>Couscous and chili</t>
+  </si>
+  <si>
+    <t>Baked cod, sauteed vegetables</t>
+  </si>
+  <si>
+    <t>Veggie bowl</t>
+  </si>
+  <si>
+    <t>Ravioli with tomato sauce</t>
+  </si>
+  <si>
+    <t>Pea crisps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Indian chicken with rice</t>
+  </si>
+  <si>
+    <t>Coffee w Half and Half</t>
+  </si>
+  <si>
+    <t>Halibut + broccoli + bread</t>
+  </si>
+  <si>
+    <t>Chicken tagine + rice</t>
+  </si>
+  <si>
+    <t>Bread 132 + nut butter (60g)</t>
+  </si>
+  <si>
+    <t>chickpeas</t>
+  </si>
+  <si>
+    <t>Eggs + kimchee</t>
+  </si>
+  <si>
+    <t>Bread + cheese</t>
+  </si>
+  <si>
+    <t>Gnocci</t>
+  </si>
+  <si>
+    <t>Rice + chicken curry</t>
+  </si>
+  <si>
+    <t>Indian bean curry  + avocado + corn chips</t>
+  </si>
+  <si>
+    <t>Pear Pumpkin Banana smoothie</t>
+  </si>
+  <si>
+    <t>Coffee w snickers</t>
+  </si>
+  <si>
+    <t>Chicken rice + curry</t>
+  </si>
+  <si>
+    <t>Bulletproof spring rolls</t>
+  </si>
+  <si>
+    <t>Bulletproof pumpkin latte</t>
+  </si>
+  <si>
+    <t>Mexican pork + frijoles</t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1603,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E662" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:E662" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E705" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:E705" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{378B7070-ADA2-F840-857A-A5C12E2181D6}" name="Start" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{50BA6A11-7F67-3245-A885-F61A29E0428D}" name="End"/>
@@ -1859,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BBD169-48D2-8F48-8801-52F9E2F03988}">
-  <dimension ref="A1:E662"/>
+  <dimension ref="A1:E705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A632" workbookViewId="0">
-      <selection activeCell="A662" sqref="A662"/>
+    <sheetView tabSelected="1" topLeftCell="A676" workbookViewId="0">
+      <selection activeCell="A706" sqref="A706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11820,6 +11889,651 @@
         <v>405</v>
       </c>
       <c r="E662" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="663" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A663" s="1">
+        <v>43766.59375</v>
+      </c>
+      <c r="C663" t="s">
+        <v>4</v>
+      </c>
+      <c r="D663" t="s">
+        <v>390</v>
+      </c>
+      <c r="E663" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="664" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A664" s="1">
+        <v>43766.510416666664</v>
+      </c>
+      <c r="C664" t="s">
+        <v>4</v>
+      </c>
+      <c r="D664" t="s">
+        <v>406</v>
+      </c>
+      <c r="E664" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="665" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A665" s="1">
+        <v>43766.770833333336</v>
+      </c>
+      <c r="C665" t="s">
+        <v>4</v>
+      </c>
+      <c r="D665" t="s">
+        <v>407</v>
+      </c>
+      <c r="E665" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="666" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A666" s="1">
+        <v>43766.729166666664</v>
+      </c>
+      <c r="C666" t="s">
+        <v>4</v>
+      </c>
+      <c r="D666" t="s">
+        <v>109</v>
+      </c>
+      <c r="E666" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="667" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A667" s="1">
+        <v>43767.270833333336</v>
+      </c>
+      <c r="C667" t="s">
+        <v>4</v>
+      </c>
+      <c r="D667" t="s">
+        <v>5</v>
+      </c>
+      <c r="E667" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="668" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A668" s="1">
+        <v>43767.3125</v>
+      </c>
+      <c r="C668" t="s">
+        <v>4</v>
+      </c>
+      <c r="D668" t="s">
+        <v>411</v>
+      </c>
+      <c r="E668" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="669" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A669" s="1">
+        <v>43767.510416666664</v>
+      </c>
+      <c r="C669" t="s">
+        <v>4</v>
+      </c>
+      <c r="D669" t="s">
+        <v>408</v>
+      </c>
+      <c r="E669" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="670" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A670" s="1">
+        <v>43767.729166666664</v>
+      </c>
+      <c r="C670" t="s">
+        <v>4</v>
+      </c>
+      <c r="D670" t="s">
+        <v>409</v>
+      </c>
+      <c r="E670" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="671" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A671" s="1">
+        <v>43767.708333333336</v>
+      </c>
+      <c r="C671" t="s">
+        <v>4</v>
+      </c>
+      <c r="D671" t="s">
+        <v>410</v>
+      </c>
+      <c r="E671" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="672" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A672" s="1">
+        <v>43766.915277777778</v>
+      </c>
+      <c r="B672" s="1">
+        <v>43767.259722222225</v>
+      </c>
+      <c r="C672" t="s">
+        <v>6</v>
+      </c>
+      <c r="E672" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.2666666667209938</v>
+      </c>
+    </row>
+    <row r="673" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A673" s="1">
+        <v>43767.928472222222</v>
+      </c>
+      <c r="B673" s="1">
+        <v>43768.24722222222</v>
+      </c>
+      <c r="C673" t="s">
+        <v>6</v>
+      </c>
+      <c r="E673" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.6499999999650754</v>
+      </c>
+    </row>
+    <row r="674" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A674" s="1">
+        <v>43768.256944444445</v>
+      </c>
+      <c r="C674" t="s">
+        <v>4</v>
+      </c>
+      <c r="D674" t="s">
+        <v>5</v>
+      </c>
+      <c r="E674" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="675" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A675" s="1">
+        <v>43769.25</v>
+      </c>
+      <c r="C675" t="s">
+        <v>4</v>
+      </c>
+      <c r="D675" t="s">
+        <v>5</v>
+      </c>
+      <c r="E675" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="676" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A676" s="1">
+        <v>43769.340277777781</v>
+      </c>
+      <c r="C676" t="s">
+        <v>4</v>
+      </c>
+      <c r="D676" t="s">
+        <v>405</v>
+      </c>
+      <c r="E676" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="677" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A677" s="1">
+        <v>43768.75</v>
+      </c>
+      <c r="C677" t="s">
+        <v>4</v>
+      </c>
+      <c r="D677" t="s">
+        <v>412</v>
+      </c>
+      <c r="E677" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="678" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A678" s="1">
+        <v>43768.645833333336</v>
+      </c>
+      <c r="C678" t="s">
+        <v>4</v>
+      </c>
+      <c r="D678" t="s">
+        <v>355</v>
+      </c>
+      <c r="E678" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="679" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A679" s="1">
+        <v>43769.416666666664</v>
+      </c>
+      <c r="C679" t="s">
+        <v>4</v>
+      </c>
+      <c r="D679" t="s">
+        <v>413</v>
+      </c>
+      <c r="E679" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="680" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A680" s="1">
+        <v>43769.809027777781</v>
+      </c>
+      <c r="C680" t="s">
+        <v>4</v>
+      </c>
+      <c r="D680" t="s">
+        <v>66</v>
+      </c>
+      <c r="E680" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="681" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A681" s="1">
+        <v>43769.770833333336</v>
+      </c>
+      <c r="C681" t="s">
+        <v>4</v>
+      </c>
+      <c r="D681" t="s">
+        <v>414</v>
+      </c>
+      <c r="E681" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="682" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A682" s="1">
+        <v>43769.541666666664</v>
+      </c>
+      <c r="C682" t="s">
+        <v>4</v>
+      </c>
+      <c r="D682" t="s">
+        <v>415</v>
+      </c>
+      <c r="E682" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="683" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A683" s="1">
+        <v>43768.959409722222</v>
+      </c>
+      <c r="B683" s="1">
+        <v>43769.240277777775</v>
+      </c>
+      <c r="C683" t="s">
+        <v>6</v>
+      </c>
+      <c r="E683" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.7408333332859911</v>
+      </c>
+    </row>
+    <row r="684" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A684" s="1">
+        <v>43769.922222222223</v>
+      </c>
+      <c r="B684" s="1">
+        <v>43770.238888888889</v>
+      </c>
+      <c r="C684" t="s">
+        <v>6</v>
+      </c>
+      <c r="E684" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.5999999999767169</v>
+      </c>
+    </row>
+    <row r="685" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A685" s="1">
+        <v>43770.354166666664</v>
+      </c>
+      <c r="C685" t="s">
+        <v>4</v>
+      </c>
+      <c r="D685" t="s">
+        <v>416</v>
+      </c>
+      <c r="E685" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="686" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A686" s="1">
+        <v>43770.6875</v>
+      </c>
+      <c r="C686" t="s">
+        <v>4</v>
+      </c>
+      <c r="D686" t="s">
+        <v>410</v>
+      </c>
+      <c r="E686" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="687" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A687" s="1">
+        <v>43771.486111111109</v>
+      </c>
+      <c r="C687" t="s">
+        <v>4</v>
+      </c>
+      <c r="D687" t="s">
+        <v>417</v>
+      </c>
+      <c r="E687" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="688" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A688" s="1">
+        <v>43771.354166666664</v>
+      </c>
+      <c r="C688" t="s">
+        <v>4</v>
+      </c>
+      <c r="D688" t="s">
+        <v>418</v>
+      </c>
+      <c r="E688" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="689" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A689" s="1">
+        <v>43770.913078703707</v>
+      </c>
+      <c r="B689" s="1">
+        <v>43771.232638888891</v>
+      </c>
+      <c r="C689" t="s">
+        <v>6</v>
+      </c>
+      <c r="E689" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.6694444444146939</v>
+      </c>
+    </row>
+    <row r="690" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A690" s="1">
+        <v>43770.854166666664</v>
+      </c>
+      <c r="C690" t="s">
+        <v>4</v>
+      </c>
+      <c r="D690" t="s">
+        <v>419</v>
+      </c>
+      <c r="E690" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="691" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A691" s="1">
+        <v>43772.012499999997</v>
+      </c>
+      <c r="B691" s="1">
+        <v>43772.231249999997</v>
+      </c>
+      <c r="C691" t="s">
+        <v>6</v>
+      </c>
+      <c r="E691" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="692" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A692" s="1">
+        <v>43771.770833333336</v>
+      </c>
+      <c r="C692" t="s">
+        <v>4</v>
+      </c>
+      <c r="D692" t="s">
+        <v>420</v>
+      </c>
+      <c r="E692" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="693" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A693" s="1">
+        <v>43771.541666666664</v>
+      </c>
+      <c r="C693" t="s">
+        <v>4</v>
+      </c>
+      <c r="D693" t="s">
+        <v>421</v>
+      </c>
+      <c r="E693" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="694" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A694" s="1">
+        <v>43772.510416666664</v>
+      </c>
+      <c r="C694" t="s">
+        <v>4</v>
+      </c>
+      <c r="D694" t="s">
+        <v>422</v>
+      </c>
+      <c r="E694" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="695" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A695" s="1">
+        <v>43772.490277777775</v>
+      </c>
+      <c r="C695" t="s">
+        <v>4</v>
+      </c>
+      <c r="D695" t="s">
+        <v>423</v>
+      </c>
+      <c r="E695" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="696" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A696" s="1">
+        <v>43772.625</v>
+      </c>
+      <c r="C696" t="s">
+        <v>4</v>
+      </c>
+      <c r="D696" t="s">
+        <v>424</v>
+      </c>
+      <c r="E696" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="697" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A697" s="1">
+        <v>43772.8125</v>
+      </c>
+      <c r="C697" t="s">
+        <v>4</v>
+      </c>
+      <c r="D697" t="s">
+        <v>425</v>
+      </c>
+      <c r="E697" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="698" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A698" s="1">
+        <v>43772.729166666664</v>
+      </c>
+      <c r="C698" t="s">
+        <v>4</v>
+      </c>
+      <c r="D698" t="s">
+        <v>426</v>
+      </c>
+      <c r="E698" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="699" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A699" s="1">
+        <v>43772.677083333336</v>
+      </c>
+      <c r="C699" t="s">
+        <v>4</v>
+      </c>
+      <c r="D699" t="s">
+        <v>427</v>
+      </c>
+      <c r="E699" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="700" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A700" s="1">
+        <v>43772.909722222219</v>
+      </c>
+      <c r="B700" s="1">
+        <v>43773.244444444441</v>
+      </c>
+      <c r="C700" t="s">
+        <v>6</v>
+      </c>
+      <c r="E700" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.0333333333255723</v>
+      </c>
+    </row>
+    <row r="701" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A701" s="1">
+        <v>43773.910416666666</v>
+      </c>
+      <c r="B701" s="1">
+        <v>43774.238888888889</v>
+      </c>
+      <c r="C701" t="s">
+        <v>6</v>
+      </c>
+      <c r="E701" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.8833333333604969</v>
+      </c>
+    </row>
+    <row r="702" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A702" s="1">
+        <v>43773.270833333336</v>
+      </c>
+      <c r="C702" t="s">
+        <v>4</v>
+      </c>
+      <c r="D702" t="s">
+        <v>241</v>
+      </c>
+      <c r="E702" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="703" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A703" s="1">
+        <v>43773.375</v>
+      </c>
+      <c r="B703" s="1">
+        <v>43773.40625</v>
+      </c>
+      <c r="C703" t="s">
+        <v>7</v>
+      </c>
+      <c r="E703" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="704" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A704" s="1">
+        <v>43773.520833333336</v>
+      </c>
+      <c r="C704" t="s">
+        <v>4</v>
+      </c>
+      <c r="D704" t="s">
+        <v>425</v>
+      </c>
+      <c r="E704" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="705" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A705" s="1">
+        <v>43773.770833333336</v>
+      </c>
+      <c r="C705" t="s">
+        <v>4</v>
+      </c>
+      <c r="D705" t="s">
+        <v>428</v>
+      </c>
+      <c r="E705" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
         <v>NA</v>
       </c>

</xml_diff>

<commit_message>
Updated data thru Nov25
</commit_message>
<xml_diff>
--- a/librelink/Rik Activity 2019.xlsx
+++ b/librelink/Rik Activity 2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc6084b92ffa451/Sprague 2019/Health 2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprague/OneDrive/Sprague 2019/Health 2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="720" documentId="114_{B7357B50-4B94-C145-ACEA-929B2CB5DE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C09E1073-8039-CF4B-9841-08FD33A31227}"/>
+  <xr:revisionPtr revIDLastSave="778" documentId="114_{B7357B50-4B94-C145-ACEA-929B2CB5DE09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{50B7FEDE-1657-9247-B166-6796B12692ED}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="1240" windowWidth="28040" windowHeight="17540" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
+    <workbookView xWindow="4980" yWindow="1120" windowWidth="28040" windowHeight="17540" xr2:uid="{EDA8406F-1EF0-334E-A61E-C477B3B92516}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="440">
   <si>
     <t>Start</t>
   </si>
@@ -1219,12 +1219,6 @@
     <t>Red Wine</t>
   </si>
   <si>
-    <t>Pasta (Pesto)</t>
-  </si>
-  <si>
-    <t>Fried chicken</t>
-  </si>
-  <si>
     <t>Salmon + mushrooms + wine</t>
   </si>
   <si>
@@ -1319,6 +1313,45 @@
   </si>
   <si>
     <t>Mexican pork + frijoles</t>
+  </si>
+  <si>
+    <t>glucose Drink (75g)</t>
+  </si>
+  <si>
+    <t>Blue muffins</t>
+  </si>
+  <si>
+    <t>Fried chicken (389g)</t>
+  </si>
+  <si>
+    <t>Banana (84g)</t>
+  </si>
+  <si>
+    <t>Pasta 437g (Pesto 122g)</t>
+  </si>
+  <si>
+    <t>banana (163g) peanut butter (167g)</t>
+  </si>
+  <si>
+    <t>Rooibus Red Tea</t>
+  </si>
+  <si>
+    <t>Chinese fried rice + mabo tofu</t>
+  </si>
+  <si>
+    <t>Apple-grape juice</t>
+  </si>
+  <si>
+    <t>apple pie (120g)</t>
+  </si>
+  <si>
+    <t>Chicken + broccoli + bread</t>
+  </si>
+  <si>
+    <t>Melotonin (3mg)</t>
+  </si>
+  <si>
+    <t>Latte (almond milk)</t>
   </si>
 </sst>
 </file>
@@ -1603,8 +1636,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E705" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:E705" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4789F44-1BF7-2E46-A5C7-20F44902F54B}" name="Table2" displayName="Table2" ref="A1:E725" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:E725" xr:uid="{B3AC50C6-9182-CB43-9817-9BF8FEE3CABC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{378B7070-ADA2-F840-857A-A5C12E2181D6}" name="Start" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{50BA6A11-7F67-3245-A885-F61A29E0428D}" name="End"/>
@@ -1928,10 +1961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BBD169-48D2-8F48-8801-52F9E2F03988}">
-  <dimension ref="A1:E705"/>
+  <dimension ref="A1:E725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A676" workbookViewId="0">
-      <selection activeCell="A706" sqref="A706"/>
+    <sheetView tabSelected="1" topLeftCell="A687" workbookViewId="0">
+      <selection activeCell="A726" sqref="A726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11391,7 +11424,7 @@
         <v>4</v>
       </c>
       <c r="D629" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E629" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11496,7 +11529,7 @@
         <v>4</v>
       </c>
       <c r="D636" t="s">
-        <v>314</v>
+        <v>432</v>
       </c>
       <c r="E636" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11556,7 +11589,7 @@
         <v>4</v>
       </c>
       <c r="D640" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E640" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11565,13 +11598,13 @@
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A641" s="1">
-        <v>43762.565972222219</v>
+        <v>43762.559027777781</v>
       </c>
       <c r="C641" t="s">
         <v>4</v>
       </c>
       <c r="D641" t="s">
-        <v>395</v>
+        <v>431</v>
       </c>
       <c r="E641" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11586,7 +11619,7 @@
         <v>4</v>
       </c>
       <c r="D642" t="s">
-        <v>85</v>
+        <v>430</v>
       </c>
       <c r="E642" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11691,7 +11724,7 @@
         <v>4</v>
       </c>
       <c r="D649" t="s">
-        <v>396</v>
+        <v>429</v>
       </c>
       <c r="E649" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11706,7 +11739,7 @@
         <v>4</v>
       </c>
       <c r="D650" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E650" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11751,7 +11784,7 @@
         <v>4</v>
       </c>
       <c r="D653" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E653" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11766,7 +11799,7 @@
         <v>4</v>
       </c>
       <c r="D654" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E654" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11796,7 +11829,7 @@
         <v>4</v>
       </c>
       <c r="D656" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E656" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11826,7 +11859,7 @@
         <v>4</v>
       </c>
       <c r="D658" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E658" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11841,7 +11874,7 @@
         <v>4</v>
       </c>
       <c r="D659" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E659" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11886,7 +11919,7 @@
         <v>4</v>
       </c>
       <c r="D662" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E662" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11916,7 +11949,7 @@
         <v>4</v>
       </c>
       <c r="D664" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E664" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11931,7 +11964,7 @@
         <v>4</v>
       </c>
       <c r="D665" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E665" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11976,7 +12009,7 @@
         <v>4</v>
       </c>
       <c r="D668" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E668" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -11991,7 +12024,7 @@
         <v>4</v>
       </c>
       <c r="D669" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E669" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12006,7 +12039,7 @@
         <v>4</v>
       </c>
       <c r="D670" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E670" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12021,7 +12054,7 @@
         <v>4</v>
       </c>
       <c r="D671" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E671" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12096,7 +12129,7 @@
         <v>4</v>
       </c>
       <c r="D676" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E676" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12111,7 +12144,7 @@
         <v>4</v>
       </c>
       <c r="D677" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E677" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12141,7 +12174,7 @@
         <v>4</v>
       </c>
       <c r="D679" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E679" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12171,7 +12204,7 @@
         <v>4</v>
       </c>
       <c r="D681" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E681" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12186,7 +12219,7 @@
         <v>4</v>
       </c>
       <c r="D682" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E682" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12231,7 +12264,7 @@
         <v>4</v>
       </c>
       <c r="D685" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E685" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12246,7 +12279,7 @@
         <v>4</v>
       </c>
       <c r="D686" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E686" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12261,7 +12294,7 @@
         <v>4</v>
       </c>
       <c r="D687" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E687" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12276,7 +12309,7 @@
         <v>4</v>
       </c>
       <c r="D688" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E688" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12306,7 +12339,7 @@
         <v>4</v>
       </c>
       <c r="D690" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E690" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12336,7 +12369,7 @@
         <v>4</v>
       </c>
       <c r="D692" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E692" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12351,7 +12384,7 @@
         <v>4</v>
       </c>
       <c r="D693" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E693" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12366,7 +12399,7 @@
         <v>4</v>
       </c>
       <c r="D694" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E694" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12381,7 +12414,7 @@
         <v>4</v>
       </c>
       <c r="D695" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E695" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12396,7 +12429,7 @@
         <v>4</v>
       </c>
       <c r="D696" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E696" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12411,7 +12444,7 @@
         <v>4</v>
       </c>
       <c r="D697" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E697" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12426,7 +12459,7 @@
         <v>4</v>
       </c>
       <c r="D698" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E698" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12441,7 +12474,7 @@
         <v>4</v>
       </c>
       <c r="D699" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E699" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12516,7 +12549,7 @@
         <v>4</v>
       </c>
       <c r="D704" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E704" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
@@ -12531,9 +12564,303 @@
         <v>4</v>
       </c>
       <c r="D705" t="s">
+        <v>426</v>
+      </c>
+      <c r="E705" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="706" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A706" s="1">
+        <v>43757.910300925927</v>
+      </c>
+      <c r="B706" s="1">
+        <v>43758.258333333331</v>
+      </c>
+      <c r="C706" t="s">
+        <v>6</v>
+      </c>
+      <c r="E706" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.3527777777053416</v>
+      </c>
+    </row>
+    <row r="707" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A707" s="1">
+        <v>43755.897256944445</v>
+      </c>
+      <c r="B707" s="25">
+        <v>43756.313194444447</v>
+      </c>
+      <c r="C707" t="s">
+        <v>6</v>
+      </c>
+      <c r="E707" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>9.9825000000419095</v>
+      </c>
+    </row>
+    <row r="708" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A708" s="1">
+        <v>43757.001701388886</v>
+      </c>
+      <c r="B708" s="1">
+        <v>43757.234722222223</v>
+      </c>
+      <c r="C708" t="s">
+        <v>6</v>
+      </c>
+      <c r="E708" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>5.5925000000861473</v>
+      </c>
+    </row>
+    <row r="709" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A709" s="1">
+        <v>43757.910300925927</v>
+      </c>
+      <c r="B709" s="1">
+        <v>43758.258333333331</v>
+      </c>
+      <c r="C709" t="s">
+        <v>6</v>
+      </c>
+      <c r="E709" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>8.3527777777053416</v>
+      </c>
+    </row>
+    <row r="710" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A710" s="1">
+        <v>43758.925694444442</v>
+      </c>
+      <c r="B710" s="1">
+        <v>43759.231944444444</v>
+      </c>
+      <c r="C710" t="s">
+        <v>6</v>
+      </c>
+      <c r="E710" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.3500000000349246</v>
+      </c>
+    </row>
+    <row r="711" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A711" s="1">
+        <v>43758.270833333336</v>
+      </c>
+      <c r="B711" s="1"/>
+      <c r="C711" t="s">
+        <v>4</v>
+      </c>
+      <c r="D711" t="s">
+        <v>427</v>
+      </c>
+      <c r="E711" s="15"/>
+    </row>
+    <row r="712" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A712" s="1">
+        <v>43757.239583333336</v>
+      </c>
+      <c r="B712" s="25"/>
+      <c r="C712" t="s">
+        <v>4</v>
+      </c>
+      <c r="D712" t="s">
         <v>428</v>
       </c>
-      <c r="E705" s="15" t="str">
+      <c r="E712" s="15"/>
+    </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A713" s="1">
+        <v>43759.618055555555</v>
+      </c>
+      <c r="B713" s="25"/>
+      <c r="C713" t="s">
+        <v>4</v>
+      </c>
+      <c r="D713" t="s">
+        <v>433</v>
+      </c>
+      <c r="E713" s="15"/>
+    </row>
+    <row r="714" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A714" s="1">
+        <v>43759.760416666664</v>
+      </c>
+      <c r="C714" t="s">
+        <v>4</v>
+      </c>
+      <c r="D714" t="s">
+        <v>419</v>
+      </c>
+      <c r="E714" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A715" s="1">
+        <v>43792.942106481481</v>
+      </c>
+      <c r="B715" s="1">
+        <v>43793.249305555553</v>
+      </c>
+      <c r="C715" t="s">
+        <v>6</v>
+      </c>
+      <c r="E715" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>7.372777777723968</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A716" s="1">
+        <v>43792.729166666664</v>
+      </c>
+      <c r="C716" t="s">
+        <v>4</v>
+      </c>
+      <c r="D716" t="s">
+        <v>434</v>
+      </c>
+      <c r="E716" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A717" s="1">
+        <v>43792.84375</v>
+      </c>
+      <c r="C717" t="s">
+        <v>4</v>
+      </c>
+      <c r="D717" t="s">
+        <v>435</v>
+      </c>
+      <c r="E717" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A718" s="1">
+        <v>43793.260416666664</v>
+      </c>
+      <c r="C718" t="s">
+        <v>4</v>
+      </c>
+      <c r="D718" t="s">
+        <v>5</v>
+      </c>
+      <c r="E718" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A719" s="1">
+        <v>43793.449305555558</v>
+      </c>
+      <c r="C719" t="s">
+        <v>4</v>
+      </c>
+      <c r="D719" t="s">
+        <v>403</v>
+      </c>
+      <c r="E719" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A720" s="1">
+        <v>43793.545138888891</v>
+      </c>
+      <c r="C720" t="s">
+        <v>4</v>
+      </c>
+      <c r="D720" t="s">
+        <v>434</v>
+      </c>
+      <c r="E720" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="721" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A721" s="1">
+        <v>43793.637499999997</v>
+      </c>
+      <c r="C721" t="s">
+        <v>4</v>
+      </c>
+      <c r="D721" t="s">
+        <v>436</v>
+      </c>
+      <c r="E721" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A722" s="1">
+        <v>43793.767361111109</v>
+      </c>
+      <c r="C722" t="s">
+        <v>4</v>
+      </c>
+      <c r="D722" t="s">
+        <v>437</v>
+      </c>
+      <c r="E722" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="723" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A723" s="1">
+        <v>43793.885416666664</v>
+      </c>
+      <c r="C723" t="s">
+        <v>4</v>
+      </c>
+      <c r="D723" t="s">
+        <v>438</v>
+      </c>
+      <c r="E723" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="724" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A724" s="1">
+        <v>43793.917361111111</v>
+      </c>
+      <c r="B724" s="1">
+        <v>43794.208333333336</v>
+      </c>
+      <c r="C724" t="s">
+        <v>6</v>
+      </c>
+      <c r="E724" s="15">
+        <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
+        <v>6.9833333333954215</v>
+      </c>
+    </row>
+    <row r="725" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A725" s="1">
+        <v>43794.21875</v>
+      </c>
+      <c r="C725" t="s">
+        <v>4</v>
+      </c>
+      <c r="D725" t="s">
+        <v>439</v>
+      </c>
+      <c r="E725" s="15" t="str">
         <f>IF(Table2[[#This Row],[Activity]]="Sleep",(Table2[[#This Row],[End]]-Table2[[#This Row],[Start]])*24,"NA")</f>
         <v>NA</v>
       </c>

</xml_diff>